<commit_message>
battleLevelConfig , footHoldConfig , spawnConfig
</commit_message>
<xml_diff>
--- a/Unity/Assets/Config/Excel/Datas/FootHold.xlsx
+++ b/Unity/Assets/Config/Excel/Datas/FootHold.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\ProjectXET\Unity\Assets\Config\Excel\Datas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A03CCB24-DFC8-4B6A-BACF-B5731BE08C50}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84FC6472-9BCE-4A3F-9A03-BC1FE7F7B8B0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="26">
   <si>
     <t>int</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -35,18 +35,6 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>##说明</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>##变量名</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>##类型</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>Id</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
@@ -120,6 +108,26 @@
   </si>
   <si>
     <t>路径5</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>##var</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>##type</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>##</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>0;0;0</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>0;0;10</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -464,10 +472,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E8"/>
+  <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F18" sqref="F18"/>
+      <selection activeCell="J12" sqref="J12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -477,30 +485,30 @@
   <sheetData>
     <row r="1" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>3</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
-        <v>4</v>
+        <v>22</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>1</v>
@@ -511,13 +519,13 @@
     </row>
     <row r="3" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
-        <v>2</v>
+        <v>23</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
@@ -525,13 +533,13 @@
         <v>1</v>
       </c>
       <c r="C4" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="E4" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
@@ -539,13 +547,13 @@
         <v>2</v>
       </c>
       <c r="C5" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="E5" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
@@ -553,13 +561,13 @@
         <v>3</v>
       </c>
       <c r="C6" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="E6" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
@@ -567,13 +575,13 @@
         <v>4</v>
       </c>
       <c r="C7" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="E7" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
@@ -581,12 +589,40 @@
         <v>5</v>
       </c>
       <c r="C8" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="E8">
+        <v>1006</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B10">
+        <v>6</v>
+      </c>
+      <c r="C10" t="s">
+        <v>16</v>
+      </c>
+      <c r="D10" t="s">
+        <v>24</v>
+      </c>
+      <c r="E10" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B11">
+        <v>7</v>
+      </c>
+      <c r="C11" t="s">
+        <v>17</v>
+      </c>
+      <c r="D11" t="s">
+        <v>25</v>
+      </c>
+      <c r="E11">
         <v>1006</v>
       </c>
     </row>

</xml_diff>